<commit_message>
Refactoring the code related to the 'currentPortfolioGoogleDrive' method
- Refactored the code related to the 'currentPortfolioGoogleDrive' method
- Solved the issue related to the opened GoogleDrive spreadsheet (avoid crash in the application)
- Reduced the number of tickers in the 'analise_fundamentalista.xlsx' spreadsheet, in order to reduce the time of processing
</commit_message>
<xml_diff>
--- a/valuation_lib/analise_fundamentalista.xlsx
+++ b/valuation_lib/analise_fundamentalista.xlsx
@@ -14,42 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>ABCB4.SA</t>
-  </si>
-  <si>
-    <t>ABEV3.SA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>BBAS3.SA</t>
   </si>
   <si>
-    <t>CIEL3.SA</t>
-  </si>
-  <si>
-    <t>CMIG3.SA</t>
-  </si>
-  <si>
-    <t>CMIG4.SA</t>
-  </si>
-  <si>
-    <t>ITSA4.SA</t>
-  </si>
-  <si>
-    <t>ITUB3.SA</t>
-  </si>
-  <si>
-    <t>ODPV3.SA</t>
-  </si>
-  <si>
     <t>PETR4.SA</t>
-  </si>
-  <si>
-    <t>USIM5.SA</t>
-  </si>
-  <si>
-    <t>WEGE3.SA</t>
   </si>
   <si>
     <t>Ticker</t>
@@ -395,7 +365,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -406,7 +376,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -419,56 +389,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <sortState ref="A2:A102">
     <sortCondition ref="A2"/>

</xml_diff>

<commit_message>
Replacing the Stocks Valuation Tool from YFinance to Status Invest scraper
- Replaced the Stocks Valuation Tool from YFinance to Status Invest scraper
- Created dedicated files to scrap data from Status Invest website:
  > status_invest.py
  > selector_bdrs.py
  > selector_etfs.py
  > selector_fiis.py
  > selector_stocks.py
  > selector_tesouro.py
- Adding the temporary folder to gitignore:
  > portfolio_lib/assets/temp
</commit_message>
<xml_diff>
--- a/valuation_lib/analise_fundamentalista.xlsx
+++ b/valuation_lib/analise_fundamentalista.xlsx
@@ -14,15 +14,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>BBAS3.SA</t>
-  </si>
-  <si>
-    <t>PETR4.SA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Ticker</t>
+  </si>
+  <si>
+    <t>Mercado</t>
+  </si>
+  <si>
+    <t>BBAS3</t>
+  </si>
+  <si>
+    <t>PETR4</t>
+  </si>
+  <si>
+    <t>AMZO34</t>
+  </si>
+  <si>
+    <t>HASH11</t>
+  </si>
+  <si>
+    <t>CPTS11</t>
+  </si>
+  <si>
+    <t>TESOURO IPCA+ 2026</t>
+  </si>
+  <si>
+    <t>Ações</t>
+  </si>
+  <si>
+    <t>BDR</t>
+  </si>
+  <si>
+    <t>ETF</t>
+  </si>
+  <si>
+    <t>FII</t>
+  </si>
+  <si>
+    <t>Tesouro Direto</t>
   </si>
 </sst>
 </file>
@@ -365,28 +395,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>